<commit_message>
Update post Second round of weighing for subsamples
</commit_message>
<xml_diff>
--- a/Raw_data/DW_subsample_DNA_CNP.xlsx
+++ b/Raw_data/DW_subsample_DNA_CNP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.uws.edu.au\dfshare\HomesCMB$\90957135\My Documents\ABS_FIRE\ABS_FIRE_MYCO\Raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://westernsydneyedu-my.sharepoint.com/personal/90957135_westernsydney_edu_au/Documents/ABS_FIRE/ABS_FIRE_MYCO/Raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDA5CCB-BB88-4E5E-B40F-C17102DEB150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{0CDA5CCB-BB88-4E5E-B40F-C17102DEB150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09DBB908-888A-47C0-A8CD-AB4B5E9B05FD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{B2F38D08-B9EC-4035-AE06-6783DCF1ABFB}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B2F38D08-B9EC-4035-AE06-6783DCF1ABFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Sample</t>
   </si>
@@ -51,9 +51,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>Total_mg</t>
-  </si>
-  <si>
     <t>Well_ID</t>
   </si>
   <si>
@@ -127,6 +124,18 @@
   </si>
   <si>
     <t>Tube_ID</t>
+  </si>
+  <si>
+    <t>B12</t>
+  </si>
+  <si>
+    <t>B11</t>
+  </si>
+  <si>
+    <t>Rough_total_mg</t>
+  </si>
+  <si>
+    <t>B10</t>
   </si>
 </sst>
 </file>
@@ -523,13 +532,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB07213B-B82F-4766-B288-8BC9F7463E0F}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -543,13 +552,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5.0999999999999996</v>
       </c>
@@ -566,18 +575,25 @@
         <v>5.5949999999999998</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5.2</v>
       </c>
+      <c r="C3">
+        <f>0.485+0.135+0.175</f>
+        <v>0.79499999999999993</v>
+      </c>
       <c r="E3">
-        <v>0.48499999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7.1</v>
       </c>
@@ -594,10 +610,10 @@
         <v>3.3820000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7.2</v>
       </c>
@@ -614,10 +630,10 @@
         <v>6.7110000000000003</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8.1</v>
       </c>
@@ -634,10 +650,10 @@
         <v>3.024</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>8.1999999999999993</v>
       </c>
@@ -648,18 +664,25 @@
         <v>0.93500000000000005</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10.1</v>
       </c>
+      <c r="C8">
+        <f>0.643+0.093+0.12</f>
+        <v>0.85599999999999998</v>
+      </c>
       <c r="E8">
         <v>0.64300000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>10.199999999999999</v>
       </c>
@@ -667,7 +690,8 @@
         <v>0.39800000000000002</v>
       </c>
       <c r="C9">
-        <v>0.89500000000000002</v>
+        <f>0.895-0.138</f>
+        <v>0.75700000000000001</v>
       </c>
       <c r="D9">
         <v>1.7889999999999999</v>
@@ -676,10 +700,10 @@
         <v>3.2050000000000001</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>11.1</v>
       </c>
@@ -696,61 +720,64 @@
         <v>5.782</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11.2</v>
       </c>
-      <c r="B11">
-        <v>0.33700000000000002</v>
-      </c>
       <c r="C11">
         <v>1.212</v>
       </c>
+      <c r="D11">
+        <f>0.337+0.088+0.075</f>
+        <v>0.5</v>
+      </c>
       <c r="E11">
         <v>1.573</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12.1</v>
       </c>
-      <c r="B12">
-        <v>0.374</v>
-      </c>
       <c r="C12">
         <v>1.4370000000000001</v>
       </c>
+      <c r="D12">
+        <f>0.374+0.147+0.094</f>
+        <v>0.61499999999999999</v>
+      </c>
       <c r="E12">
         <v>1.829</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12.2</v>
       </c>
-      <c r="B13">
-        <v>0.432</v>
-      </c>
       <c r="C13">
         <v>1.2709999999999999</v>
       </c>
+      <c r="D13">
+        <f>0.432+0.129+0.224</f>
+        <v>0.78499999999999992</v>
+      </c>
       <c r="E13">
         <v>1.7310000000000001</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>26.1</v>
       </c>
@@ -767,10 +794,10 @@
         <v>3.5670000000000002</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>26.2</v>
       </c>
@@ -787,35 +814,42 @@
         <v>4.0780000000000003</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>29.1</v>
       </c>
-      <c r="B16">
-        <v>0.41699999999999998</v>
-      </c>
       <c r="C16">
         <v>1.571</v>
       </c>
+      <c r="D16">
+        <f>0.417+0.2</f>
+        <v>0.61699999999999999</v>
+      </c>
       <c r="E16">
         <v>2.0289999999999999</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>29.2</v>
       </c>
+      <c r="C17">
+        <v>0.34200000000000003</v>
+      </c>
       <c r="E17">
         <v>0.34200000000000003</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>31.1</v>
       </c>
@@ -826,16 +860,17 @@
         <v>0.92200000000000004</v>
       </c>
       <c r="D18">
+        <f>2.027</f>
         <v>2.0270000000000001</v>
       </c>
       <c r="E18">
         <v>3.1930000000000001</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>31.2</v>
       </c>
@@ -852,10 +887,10 @@
         <v>5.9139999999999997</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>34.1</v>
       </c>
@@ -872,10 +907,10 @@
         <v>5.3390000000000004</v>
       </c>
       <c r="F20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>34.200000000000003</v>
       </c>
@@ -892,10 +927,10 @@
         <v>4.165</v>
       </c>
       <c r="F21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>49.1</v>
       </c>
@@ -909,10 +944,10 @@
         <v>2.714</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>49.2</v>
       </c>
@@ -926,10 +961,10 @@
         <v>2.23</v>
       </c>
       <c r="F23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>56.1</v>
       </c>
@@ -946,24 +981,25 @@
         <v>3.2530000000000001</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>56.2</v>
       </c>
-      <c r="B25">
-        <v>0.44400000000000001</v>
-      </c>
       <c r="C25">
         <v>1.093</v>
       </c>
+      <c r="D25">
+        <f>0.44+0.126</f>
+        <v>0.56600000000000006</v>
+      </c>
       <c r="E25">
         <v>1.5489999999999999</v>
       </c>
       <c r="F25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -976,27 +1012,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3E5F06F-C747-40AB-9C83-C499E0866673}">
   <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1010,7 +1046,7 @@
         <v>0.96799999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1026,7 +1062,7 @@
         <v>0.86199999999999988</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1040,7 +1076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1054,7 +1090,7 @@
         <v>2.556</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1068,7 +1104,7 @@
         <v>0.876</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1082,7 +1118,7 @@
         <v>0.26500000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1096,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1110,7 +1146,7 @@
         <v>0.24399999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1124,7 +1160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1138,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1152,27 +1188,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <f>SUM(C13:D13)</f>
-        <v>2.641</v>
+        <f t="shared" ref="B13:B39" si="0">SUM(C13:D13)</f>
+        <v>2.6410000000000005</v>
       </c>
       <c r="C13" s="1">
-        <v>0.42499999999999999</v>
+        <f>0.425-0.2</f>
+        <v>0.22499999999999998</v>
       </c>
       <c r="D13" s="1">
-        <v>2.2160000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+        <f>2.216+0.2</f>
+        <v>2.4160000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <f>SUM(C14:D14)</f>
+        <f t="shared" si="0"/>
         <v>3.5700000000000003</v>
       </c>
       <c r="C14" s="1">
@@ -1182,12 +1220,12 @@
         <v>3.0880000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <f>SUM(C15:D15)</f>
+        <f t="shared" si="0"/>
         <v>0.61899999999999999</v>
       </c>
       <c r="C15" s="1">
@@ -1197,12 +1235,12 @@
         <v>0.247</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <f>SUM(C16:D16)</f>
+        <f t="shared" si="0"/>
         <v>1.9770000000000001</v>
       </c>
       <c r="C16" s="1">
@@ -1212,12 +1250,12 @@
         <v>1.524</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <f>SUM(C17:D17)</f>
+        <f t="shared" si="0"/>
         <v>1.484</v>
       </c>
       <c r="C17" s="1">
@@ -1227,12 +1265,12 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <f>SUM(C18:D18)</f>
+        <f t="shared" si="0"/>
         <v>0.91700000000000004</v>
       </c>
       <c r="C18" s="1">
@@ -1242,12 +1280,12 @@
         <v>0.48699999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <f>SUM(C19:D19)</f>
+        <f t="shared" si="0"/>
         <v>2.4210000000000003</v>
       </c>
       <c r="C19" s="1">
@@ -1257,12 +1295,12 @@
         <v>1.923</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <f>SUM(C20:D20)</f>
+        <f t="shared" si="0"/>
         <v>0.748</v>
       </c>
       <c r="C20" s="1">
@@ -1272,12 +1310,12 @@
         <v>0.32500000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <f>SUM(C21:D21)</f>
+        <f t="shared" si="0"/>
         <v>1.6079999999999999</v>
       </c>
       <c r="C21" s="1">
@@ -1287,12 +1325,12 @@
         <v>1.1779999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <f>SUM(C22:D22)</f>
+        <f t="shared" si="0"/>
         <v>1.143</v>
       </c>
       <c r="C22" s="1">
@@ -1302,12 +1340,12 @@
         <v>0.74299999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <f>SUM(C23:D23)</f>
+        <f t="shared" si="0"/>
         <v>2.032</v>
       </c>
       <c r="C23" s="1">
@@ -1317,12 +1355,12 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <f>SUM(C24:D24)</f>
+        <f t="shared" si="0"/>
         <v>1.0030000000000001</v>
       </c>
       <c r="C24" s="1">
@@ -1332,12 +1370,12 @@
         <v>0.61599999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <f>SUM(C25:D25)</f>
+        <f t="shared" si="0"/>
         <v>1.9450000000000001</v>
       </c>
       <c r="C25" s="1">
@@ -1347,12 +1385,12 @@
         <v>1.514</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <f>SUM(C26:D26)</f>
+        <f t="shared" si="0"/>
         <v>3.625</v>
       </c>
       <c r="C26" s="1">
@@ -1362,12 +1400,12 @@
         <v>3.2170000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <f>SUM(C27:D27)</f>
+        <f t="shared" si="0"/>
         <v>1.0979999999999999</v>
       </c>
       <c r="C27" s="1">
@@ -1377,12 +1415,12 @@
         <v>0.59699999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <f>SUM(C28:D28)</f>
+        <f t="shared" si="0"/>
         <v>0.46899999999999997</v>
       </c>
       <c r="C28" s="1">
@@ -1392,24 +1430,24 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <f>SUM(C29:D29)</f>
+        <f t="shared" si="0"/>
         <v>0.308</v>
       </c>
       <c r="C29" s="1">
         <v>0.308</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <f>SUM(C30:D30)</f>
+        <f t="shared" si="0"/>
         <v>3.093</v>
       </c>
       <c r="C30" s="1">
@@ -1419,12 +1457,12 @@
         <v>2.6789999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>31</v>
       </c>
       <c r="B31" s="1">
-        <f>SUM(C31:D31)</f>
+        <f t="shared" si="0"/>
         <v>0.88600000000000001</v>
       </c>
       <c r="C31" s="1">
@@ -1434,12 +1472,12 @@
         <v>0.45700000000000002</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>32</v>
       </c>
       <c r="B32" s="1">
-        <f>SUM(C32:D32)</f>
+        <f t="shared" si="0"/>
         <v>1.319</v>
       </c>
       <c r="C32" s="1">
@@ -1449,12 +1487,12 @@
         <v>0.91200000000000003</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>33</v>
       </c>
       <c r="B33" s="1">
-        <f>SUM(C33:D33)</f>
+        <f t="shared" si="0"/>
         <v>1.054</v>
       </c>
       <c r="C33" s="1">
@@ -1464,12 +1502,12 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>34</v>
       </c>
       <c r="B34" s="1">
-        <f>SUM(C34:D34)</f>
+        <f t="shared" si="0"/>
         <v>3.0369999999999999</v>
       </c>
       <c r="C34" s="1">
@@ -1479,12 +1517,12 @@
         <v>2.6539999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>35</v>
       </c>
       <c r="B35" s="1">
-        <f>SUM(C35:D35)</f>
+        <f t="shared" si="0"/>
         <v>1.069</v>
       </c>
       <c r="C35" s="1">
@@ -1494,12 +1532,12 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>36</v>
       </c>
       <c r="B36" s="1">
-        <f>SUM(C36:D36)</f>
+        <f t="shared" si="0"/>
         <v>1.171</v>
       </c>
       <c r="C36" s="1">
@@ -1509,24 +1547,24 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>37</v>
       </c>
       <c r="B37" s="1">
-        <f>SUM(C37:D37)</f>
+        <f t="shared" si="0"/>
         <v>0.157</v>
       </c>
       <c r="D37" s="1">
         <v>0.157</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>38</v>
       </c>
       <c r="B38" s="1">
-        <f>SUM(C38:D38)</f>
+        <f t="shared" si="0"/>
         <v>0.21</v>
       </c>
       <c r="C38" s="1">
@@ -1534,12 +1572,12 @@
       </c>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>39</v>
       </c>
       <c r="B39" s="1">
-        <f>SUM(C39:D39)</f>
+        <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="C39" s="1">
@@ -1547,19 +1585,21 @@
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>40</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1">
-        <v>0.437</v>
+        <f>0.437-0.12</f>
+        <v>0.317</v>
       </c>
       <c r="D40" s="1">
-        <v>0.46200000000000002</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+        <f>0.462+0.12</f>
+        <v>0.58200000000000007</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>41</v>
       </c>
@@ -1571,17 +1611,20 @@
         <v>0.313</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>42</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1">
-        <v>0.55700000000000005</v>
-      </c>
-      <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+        <f>0.557-0.093</f>
+        <v>0.46400000000000008</v>
+      </c>
+      <c r="D42" s="1">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>43</v>
       </c>
@@ -1591,7 +1634,7 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>44</v>
       </c>
@@ -1601,19 +1644,21 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>45</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1">
-        <v>0.41899999999999998</v>
+        <f>0.419-0.147</f>
+        <v>0.27200000000000002</v>
       </c>
       <c r="D45" s="1">
-        <v>0.55100000000000005</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+        <f>0.551+0.147</f>
+        <v>0.69800000000000006</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>46</v>
       </c>
@@ -1625,7 +1670,7 @@
         <v>0.61599999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>47</v>
       </c>
@@ -1635,7 +1680,7 @@
       </c>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>48</v>
       </c>
@@ -1645,19 +1690,21 @@
       </c>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>49</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="2">
-        <v>0.39800000000000002</v>
+        <f>0.398-0.094</f>
+        <v>0.30400000000000005</v>
       </c>
       <c r="D49" s="1">
-        <v>1.3879999999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+        <f>1.388+0.094</f>
+        <v>1.482</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>50</v>
       </c>
@@ -1669,7 +1716,7 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>51</v>
       </c>
@@ -1681,7 +1728,7 @@
         <v>1.0389999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>52</v>
       </c>
@@ -1693,7 +1740,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>53</v>
       </c>
@@ -1705,19 +1752,21 @@
         <v>1.091</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>54</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1">
-        <v>0.41099999999999998</v>
+        <f>0.411-0.129</f>
+        <v>0.28199999999999997</v>
       </c>
       <c r="D54" s="1">
-        <v>0.27700000000000002</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+        <f>0.277+0.129</f>
+        <v>0.40600000000000003</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>55</v>
       </c>
@@ -1729,7 +1778,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>56</v>
       </c>
@@ -1741,7 +1790,7 @@
         <v>0.50600000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>57</v>
       </c>
@@ -1753,7 +1802,7 @@
         <v>0.34599999999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>58</v>
       </c>
@@ -1765,7 +1814,7 @@
         <v>0.59199999999999997</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>59</v>
       </c>
@@ -1777,7 +1826,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>60</v>
       </c>
@@ -1789,7 +1838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>61</v>
       </c>
@@ -1799,7 +1848,7 @@
       </c>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>62</v>
       </c>
@@ -1811,7 +1860,7 @@
         <v>0.50600000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>63</v>
       </c>
@@ -1823,7 +1872,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>64</v>
       </c>
@@ -1833,7 +1882,7 @@
       </c>
       <c r="D64" s="1"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>65</v>
       </c>
@@ -1845,7 +1894,7 @@
         <v>0.72299999999999998</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>66</v>
       </c>
@@ -1857,7 +1906,7 @@
         <v>3.0409999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>67</v>
       </c>
@@ -1869,29 +1918,34 @@
         <v>0.81200000000000006</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>68</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1">
-        <v>0.46100000000000002</v>
+        <f>0.461-0.224</f>
+        <v>0.23700000000000002</v>
       </c>
       <c r="D68" s="1">
-        <v>0.50600000000000001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+        <f>0.506+0.224</f>
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>69</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1">
-        <v>0.434</v>
-      </c>
-      <c r="D69" s="1"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+        <f>0.434-0.125</f>
+        <v>0.309</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>70</v>
       </c>
@@ -1901,7 +1955,7 @@
       </c>
       <c r="D70" s="1"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>71</v>
       </c>
@@ -1911,7 +1965,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>72</v>
       </c>
@@ -1923,7 +1977,7 @@
         <v>0.55400000000000005</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>73</v>
       </c>
@@ -1935,7 +1989,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>74</v>
       </c>
@@ -1947,7 +2001,7 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>75</v>
       </c>
@@ -1959,7 +2013,7 @@
         <v>0.90900000000000003</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>76</v>
       </c>
@@ -1971,7 +2025,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>77</v>
       </c>
@@ -1983,19 +2037,21 @@
         <v>4.03</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>78</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1">
-        <v>0.42899999999999999</v>
+        <f>0.429-0.135</f>
+        <v>0.29399999999999998</v>
       </c>
       <c r="D78" s="1">
-        <v>0.24099999999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+        <f>0.241+0.135</f>
+        <v>0.376</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>79</v>
       </c>
@@ -2007,19 +2063,21 @@
         <v>2.4889999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>80</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1">
-        <v>0.40600000000000003</v>
+        <f>0.406-0.172</f>
+        <v>0.23400000000000004</v>
       </c>
       <c r="D80" s="1">
-        <v>0.14099999999999999</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+        <f>0.141+0.172</f>
+        <v>0.31299999999999994</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>81</v>
       </c>
@@ -2029,7 +2087,7 @@
       </c>
       <c r="D81" s="1"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>82</v>
       </c>
@@ -2041,7 +2099,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>83</v>
       </c>
@@ -2053,7 +2111,7 @@
         <v>2.1179999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>84</v>
       </c>
@@ -2065,7 +2123,7 @@
         <v>1.833</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>85</v>
       </c>
@@ -2075,7 +2133,7 @@
       </c>
       <c r="D85" s="1"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>86</v>
       </c>
@@ -2087,7 +2145,7 @@
         <v>0.41899999999999998</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>87</v>
       </c>
@@ -2099,7 +2157,7 @@
         <v>0.57399999999999995</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>88</v>
       </c>
@@ -2111,7 +2169,7 @@
         <v>0.52600000000000002</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>89</v>
       </c>
@@ -2121,7 +2179,7 @@
       </c>
       <c r="D89" s="1"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>90</v>
       </c>
@@ -2132,7 +2190,7 @@
         <v>3.653</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>91</v>
       </c>
@@ -2143,7 +2201,7 @@
         <v>2.7530000000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>92</v>
       </c>
@@ -2151,7 +2209,7 @@
         <v>0.58199999999999996</v>
       </c>
     </row>
-    <row r="93" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>93</v>
       </c>
@@ -2162,7 +2220,7 @@
         <v>0.36499999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>94</v>
       </c>
@@ -2173,35 +2231,39 @@
         <v>2.8050000000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>95</v>
       </c>
       <c r="C95" s="2">
-        <v>0.40600000000000003</v>
+        <f>0.406-0.088</f>
+        <v>0.31800000000000006</v>
       </c>
       <c r="D95">
-        <v>0.91300000000000003</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+        <f>0.913+0.088</f>
+        <v>1.0010000000000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>96</v>
       </c>
       <c r="C96" s="2">
-        <v>0.40300000000000002</v>
+        <f>0.403-0.075</f>
+        <v>0.32800000000000001</v>
       </c>
       <c r="D96">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+        <f>0.24+0.075</f>
+        <v>0.315</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99" s="1"/>
     </row>
   </sheetData>

</xml_diff>